<commit_message>
data/schedules/Schedule 2025 - 2026.xlsx
</commit_message>
<xml_diff>
--- a/data/schedules/Schedule 2025 - 2026.xlsx
+++ b/data/schedules/Schedule 2025 - 2026.xlsx
@@ -46,6 +46,9 @@
     <t>2025-10-26</t>
   </si>
   <si>
+    <t>Gail and Larry Nader</t>
+  </si>
+  <si>
     <t>2025-11-23</t>
   </si>
   <si>
@@ -74,9 +77,6 @@
   </si>
   <si>
     <t>2026-04-26</t>
-  </si>
-  <si>
-    <t>Betty Yarris</t>
   </si>
   <si>
     <t>Sue and Dave Potter</t>
@@ -280,10 +280,10 @@
     <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1402,23 +1402,25 @@
       <c r="B4" t="s" s="8">
         <v>10</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="C4" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="7">
         <v>11</v>
       </c>
       <c r="B5" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="E5" t="s" s="10">
+      <c r="C5" s="10"/>
+      <c r="D5" t="s" s="9">
         <v>13</v>
+      </c>
+      <c r="E5" t="s" s="9">
+        <v>14</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
@@ -1426,54 +1428,52 @@
         <v>12</v>
       </c>
       <c r="B6" t="s" s="8">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s" s="10">
         <v>15</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="C6" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="7">
         <v>13</v>
       </c>
       <c r="B7" t="s" s="8">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="C7" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="7">
         <v>14</v>
       </c>
       <c r="B8" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s" s="10">
         <v>19</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="C8" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="7">
         <v>15</v>
       </c>
       <c r="B9" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="D9" t="s" s="10">
+      <c r="C9" s="10"/>
+      <c r="D9" t="s" s="9">
         <v>22</v>
       </c>
-      <c r="E9" t="s" s="10">
+      <c r="E9" t="s" s="9">
         <v>23</v>
       </c>
     </row>
@@ -1484,9 +1484,9 @@
       <c r="B10" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>